<commit_message>
modifying and editing the single T maze code and making csv file for the first day of training
</commit_message>
<xml_diff>
--- a/src/omniroute_operation/src/single_T_maze/Training_Trials .xlsx
+++ b/src/omniroute_operation/src/single_T_maze/Training_Trials .xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="245" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="245" uniqueCount="10">
   <si>
     <t xml:space="preserve">Left_Cue</t>
   </si>
@@ -49,25 +49,6 @@
     <t xml:space="preserve">forced_choice</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">forced_</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">choice</t>
-    </r>
-  </si>
-  <si>
     <t xml:space="preserve">Black</t>
   </si>
 </sst>
@@ -78,7 +59,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="10">
+  <fonts count="7">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -115,28 +96,11 @@
       <charset val="1"/>
     </font>
     <font>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -181,7 +145,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="5">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -199,18 +163,6 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -233,11 +185,11 @@
   </sheetPr>
   <dimension ref="A1:E79"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="250" zoomScaleNormal="250" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F3" activeCellId="0" sqref="F3"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A28" colorId="64" zoomScale="250" zoomScaleNormal="250" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G55" activeCellId="0" sqref="G55"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.859375" defaultRowHeight="13" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.875" defaultRowHeight="13" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="5" min="5" style="0" width="11.71"/>
   </cols>
@@ -274,7 +226,7 @@
       </c>
       <c r="E2" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.703728160433975</v>
+        <v>0.325341825288847</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -284,15 +236,15 @@
       <c r="B3" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C3" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="D3" s="5" t="s">
-        <v>9</v>
+      <c r="C3" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>8</v>
       </c>
       <c r="E3" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.68315721817932</v>
+        <v>0.736949194848838</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -302,69 +254,69 @@
       <c r="B4" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="D4" s="5" t="s">
-        <v>9</v>
+      <c r="C4" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>8</v>
       </c>
       <c r="E4" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.91112092037946</v>
+        <v>0.76950926060755</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C5" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="D5" s="5" t="s">
-        <v>9</v>
+        <v>5</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>8</v>
       </c>
       <c r="E5" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.862919104472976</v>
+        <v>0.198476696039102</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C6" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="D6" s="5" t="s">
-        <v>9</v>
+        <v>5</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>8</v>
       </c>
       <c r="E6" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.275609655010023</v>
+        <v>0.572876886956201</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C7" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="D7" s="5" t="s">
-        <v>9</v>
+        <v>5</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>8</v>
       </c>
       <c r="E7" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.193600986261705</v>
+        <v>0.14124046393787</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -374,15 +326,15 @@
       <c r="B8" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C8" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="D8" s="5" t="s">
-        <v>9</v>
+      <c r="C8" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>8</v>
       </c>
       <c r="E8" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.388707142039832</v>
+        <v>0.349876633085204</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -395,12 +347,12 @@
       <c r="C9" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="D9" s="5" t="s">
-        <v>9</v>
+      <c r="D9" s="1" t="s">
+        <v>8</v>
       </c>
       <c r="E9" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.8898837849441</v>
+        <v>0.859936170081302</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -410,15 +362,15 @@
       <c r="B10" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C10" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="D10" s="5" t="s">
-        <v>9</v>
+      <c r="C10" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>8</v>
       </c>
       <c r="E10" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.712689436168145</v>
+        <v>0.0333754070501721</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -428,7 +380,7 @@
       <c r="B11" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C11" s="4" t="s">
+      <c r="C11" s="3" t="s">
         <v>7</v>
       </c>
       <c r="D11" s="1" t="s">
@@ -436,7 +388,7 @@
       </c>
       <c r="E11" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.701103725940792</v>
+        <v>0.210536406038008</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -446,15 +398,15 @@
       <c r="B12" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C12" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="D12" s="5" t="s">
-        <v>9</v>
+      <c r="C12" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>8</v>
       </c>
       <c r="E12" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.251746514208332</v>
+        <v>0.817265043890606</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -464,15 +416,15 @@
       <c r="B13" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C13" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="D13" s="5" t="s">
-        <v>9</v>
+      <c r="C13" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>8</v>
       </c>
       <c r="E13" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.00771700734842541</v>
+        <v>0.285758522491754</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -482,15 +434,15 @@
       <c r="B14" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C14" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="D14" s="5" t="s">
-        <v>9</v>
+      <c r="C14" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>8</v>
       </c>
       <c r="E14" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.34416299842353</v>
+        <v>0.0380000034580211</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -500,15 +452,15 @@
       <c r="B15" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C15" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="D15" s="5" t="s">
-        <v>9</v>
+      <c r="C15" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>8</v>
       </c>
       <c r="E15" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.868552508149578</v>
+        <v>0.906227525004015</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -521,12 +473,12 @@
       <c r="C16" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="D16" s="5" t="s">
-        <v>9</v>
+      <c r="D16" s="1" t="s">
+        <v>8</v>
       </c>
       <c r="E16" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.308681683008814</v>
+        <v>0.32416219018021</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -536,15 +488,15 @@
       <c r="B17" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C17" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="D17" s="5" t="s">
-        <v>9</v>
+      <c r="C17" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>8</v>
       </c>
       <c r="E17" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.838049142948817</v>
+        <v>0.805858717578101</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -554,15 +506,15 @@
       <c r="B18" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C18" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="D18" s="5" t="s">
-        <v>9</v>
+      <c r="C18" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>8</v>
       </c>
       <c r="E18" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.192813842256341</v>
+        <v>0.561488343663837</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -572,15 +524,15 @@
       <c r="B19" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C19" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="D19" s="5" t="s">
-        <v>9</v>
+      <c r="C19" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>8</v>
       </c>
       <c r="E19" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.745249043172279</v>
+        <v>0.210259245844799</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -590,7 +542,7 @@
       <c r="B20" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C20" s="4" t="s">
+      <c r="C20" s="3" t="s">
         <v>7</v>
       </c>
       <c r="D20" s="1" t="s">
@@ -598,7 +550,7 @@
       </c>
       <c r="E20" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.383356475127992</v>
+        <v>0.715537780200506</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -608,15 +560,15 @@
       <c r="B21" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C21" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="D21" s="5" t="s">
-        <v>9</v>
+      <c r="C21" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>8</v>
       </c>
       <c r="E21" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.710068583751356</v>
+        <v>0.679905647113464</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -626,15 +578,15 @@
       <c r="B22" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C22" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="D22" s="5" t="s">
-        <v>9</v>
+      <c r="C22" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>8</v>
       </c>
       <c r="E22" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.613268463156387</v>
+        <v>0.705341658699668</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -647,12 +599,12 @@
       <c r="C23" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="D23" s="5" t="s">
-        <v>9</v>
+      <c r="D23" s="1" t="s">
+        <v>8</v>
       </c>
       <c r="E23" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.745155270051798</v>
+        <v>0.900037112859407</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -662,69 +614,69 @@
       <c r="B24" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C24" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="D24" s="5" t="s">
-        <v>9</v>
+      <c r="C24" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>8</v>
       </c>
       <c r="E24" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.813425454424158</v>
+        <v>0.738065161912534</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C25" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="D25" s="5" t="s">
-        <v>9</v>
+        <v>6</v>
+      </c>
+      <c r="C25" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>8</v>
       </c>
       <c r="E25" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.955062935602156</v>
+        <v>0.298767366707625</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C26" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="D26" s="5" t="s">
-        <v>9</v>
+        <v>6</v>
+      </c>
+      <c r="C26" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>8</v>
       </c>
       <c r="E26" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.564690361663498</v>
+        <v>0.0248798426137125</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C27" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="D27" s="5" t="s">
-        <v>9</v>
+        <v>6</v>
+      </c>
+      <c r="C27" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>8</v>
       </c>
       <c r="E27" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.775977273888789</v>
+        <v>0.361025096301436</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -734,25 +686,25 @@
       <c r="B28" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C28" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="D28" s="5" t="s">
-        <v>9</v>
+      <c r="C28" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D28" s="1" t="s">
+        <v>8</v>
       </c>
       <c r="E28" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.652783801005377</v>
+        <v>0.463477879596986</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C29" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C29" s="3" t="s">
         <v>7</v>
       </c>
       <c r="D29" s="1" t="s">
@@ -760,25 +712,25 @@
       </c>
       <c r="E29" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.657332054405596</v>
+        <v>0.899677576848432</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C30" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="D30" s="5" t="s">
-        <v>9</v>
+      <c r="D30" s="1" t="s">
+        <v>8</v>
       </c>
       <c r="E30" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.597892245066648</v>
+        <v>0.17486489363463</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -788,15 +740,15 @@
       <c r="B31" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C31" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="D31" s="5" t="s">
-        <v>9</v>
+      <c r="C31" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D31" s="1" t="s">
+        <v>8</v>
       </c>
       <c r="E31" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.754912355426012</v>
+        <v>0.919198393139249</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -806,15 +758,15 @@
       <c r="B32" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C32" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="D32" s="5" t="s">
-        <v>9</v>
+      <c r="C32" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D32" s="1" t="s">
+        <v>8</v>
       </c>
       <c r="E32" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.230800727919324</v>
+        <v>0.932599751045215</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -824,15 +776,15 @@
       <c r="B33" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C33" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="D33" s="5" t="s">
-        <v>9</v>
+      <c r="C33" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D33" s="1" t="s">
+        <v>8</v>
       </c>
       <c r="E33" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.99047874057445</v>
+        <v>0.687349431227975</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -842,15 +794,15 @@
       <c r="B34" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C34" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="D34" s="5" t="s">
-        <v>9</v>
+      <c r="C34" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D34" s="1" t="s">
+        <v>8</v>
       </c>
       <c r="E34" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.0740618163482462</v>
+        <v>0.668866102360497</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -860,15 +812,15 @@
       <c r="B35" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C35" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="D35" s="5" t="s">
-        <v>9</v>
+      <c r="C35" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D35" s="1" t="s">
+        <v>8</v>
       </c>
       <c r="E35" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.556824635690992</v>
+        <v>0.299113711228443</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -878,15 +830,15 @@
       <c r="B36" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C36" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="D36" s="5" t="s">
-        <v>9</v>
+      <c r="C36" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D36" s="1" t="s">
+        <v>8</v>
       </c>
       <c r="E36" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.670353898028697</v>
+        <v>0.253136182277389</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -896,15 +848,15 @@
       <c r="B37" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C37" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="D37" s="5" t="s">
-        <v>9</v>
+      <c r="C37" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D37" s="1" t="s">
+        <v>8</v>
       </c>
       <c r="E37" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.138615125794809</v>
+        <v>0.978108447662928</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -914,15 +866,15 @@
       <c r="B38" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C38" s="7" t="s">
-        <v>10</v>
+      <c r="C38" s="4" t="s">
+        <v>9</v>
       </c>
       <c r="D38" s="1" t="s">
         <v>8</v>
       </c>
       <c r="E38" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.143636887872473</v>
+        <v>0.350758258224709</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -932,15 +884,15 @@
       <c r="B39" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C39" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="D39" s="5" t="s">
-        <v>9</v>
+      <c r="C39" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D39" s="1" t="s">
+        <v>8</v>
       </c>
       <c r="E39" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.140349001838553</v>
+        <v>0.530027475603528</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -950,15 +902,15 @@
       <c r="B40" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C40" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="D40" s="5" t="s">
-        <v>9</v>
+      <c r="C40" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D40" s="1" t="s">
+        <v>8</v>
       </c>
       <c r="E40" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.700154555287471</v>
+        <v>0.0932446401893503</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -968,15 +920,15 @@
       <c r="B41" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C41" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="D41" s="5" t="s">
-        <v>9</v>
+      <c r="C41" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D41" s="1" t="s">
+        <v>8</v>
       </c>
       <c r="E41" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.589976218695945</v>
+        <v>0.00586027250121808</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -986,15 +938,15 @@
       <c r="B42" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C42" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="D42" s="5" t="s">
-        <v>9</v>
+      <c r="C42" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D42" s="1" t="s">
+        <v>8</v>
       </c>
       <c r="E42" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.628731882530868</v>
+        <v>0.134216457692807</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1004,15 +956,15 @@
       <c r="B43" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C43" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="D43" s="5" t="s">
-        <v>9</v>
+      <c r="C43" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D43" s="1" t="s">
+        <v>8</v>
       </c>
       <c r="E43" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.323978006194974</v>
+        <v>0.807968323442944</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1022,15 +974,15 @@
       <c r="B44" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C44" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="D44" s="5" t="s">
-        <v>9</v>
+      <c r="C44" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D44" s="1" t="s">
+        <v>8</v>
       </c>
       <c r="E44" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.637354861051604</v>
+        <v>0.867169010774887</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1040,15 +992,15 @@
       <c r="B45" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C45" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="D45" s="5" t="s">
-        <v>9</v>
+      <c r="C45" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D45" s="1" t="s">
+        <v>8</v>
       </c>
       <c r="E45" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.27920794858555</v>
+        <v>0.736377004438553</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1058,51 +1010,51 @@
       <c r="B46" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C46" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="D46" s="5" t="s">
-        <v>9</v>
+      <c r="C46" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D46" s="1" t="s">
+        <v>8</v>
       </c>
       <c r="E46" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.240721888717913</v>
+        <v>0.0754379602488955</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C47" s="7" t="s">
-        <v>10</v>
+        <v>6</v>
+      </c>
+      <c r="C47" s="4" t="s">
+        <v>9</v>
       </c>
       <c r="D47" s="1" t="s">
         <v>8</v>
       </c>
       <c r="E47" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.927361098609358</v>
+        <v>0.650459452788075</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C48" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="D48" s="5" t="s">
-        <v>9</v>
+        <v>6</v>
+      </c>
+      <c r="C48" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D48" s="1" t="s">
+        <v>8</v>
       </c>
       <c r="E48" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.733983773286755</v>
+        <v>0.907833678001237</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1112,15 +1064,15 @@
       <c r="B49" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C49" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="D49" s="5" t="s">
-        <v>9</v>
+      <c r="C49" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D49" s="1" t="s">
+        <v>8</v>
       </c>
       <c r="E49" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.997473521896128</v>
+        <v>0.885722060330212</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1130,15 +1082,15 @@
       <c r="B50" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C50" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="D50" s="5" t="s">
-        <v>9</v>
+      <c r="C50" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D50" s="1" t="s">
+        <v>8</v>
       </c>
       <c r="E50" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.811673965691375</v>
+        <v>0.78925459966701</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1148,15 +1100,15 @@
       <c r="B51" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C51" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="D51" s="5" t="s">
-        <v>9</v>
+      <c r="C51" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D51" s="1" t="s">
+        <v>8</v>
       </c>
       <c r="E51" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.0191105146953704</v>
+        <v>0.582980643174923</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1166,51 +1118,51 @@
       <c r="B52" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C52" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="D52" s="5" t="s">
-        <v>9</v>
+      <c r="C52" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D52" s="1" t="s">
+        <v>8</v>
       </c>
       <c r="E52" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.850703835528354</v>
+        <v>0.992398338876803</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B53" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C53" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="D53" s="5" t="s">
-        <v>9</v>
+        <v>6</v>
+      </c>
+      <c r="C53" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D53" s="1" t="s">
+        <v>8</v>
       </c>
       <c r="E53" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.32723552166557</v>
+        <v>0.224072444476191</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C54" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="D54" s="5" t="s">
-        <v>9</v>
+        <v>6</v>
+      </c>
+      <c r="C54" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D54" s="1" t="s">
+        <v>8</v>
       </c>
       <c r="E54" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.517399153460635</v>
+        <v>0.483531593234427</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1220,15 +1172,15 @@
       <c r="B55" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C55" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="D55" s="5" t="s">
-        <v>9</v>
+      <c r="C55" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D55" s="1" t="s">
+        <v>8</v>
       </c>
       <c r="E55" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.212231267891618</v>
+        <v>0.670818653005099</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1238,15 +1190,15 @@
       <c r="B56" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C56" s="6" t="s">
-        <v>10</v>
+      <c r="C56" s="4" t="s">
+        <v>9</v>
       </c>
       <c r="D56" s="1" t="s">
         <v>8</v>
       </c>
       <c r="E56" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.254933742034375</v>
+        <v>0.862101870153993</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1256,51 +1208,51 @@
       <c r="B57" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C57" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="D57" s="5" t="s">
-        <v>9</v>
+      <c r="C57" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D57" s="1" t="s">
+        <v>8</v>
       </c>
       <c r="E57" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.589140341989797</v>
+        <v>0.289151210477785</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B58" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C58" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="D58" s="5" t="s">
-        <v>9</v>
+        <v>5</v>
+      </c>
+      <c r="C58" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D58" s="1" t="s">
+        <v>8</v>
       </c>
       <c r="E58" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.949211715670042</v>
+        <v>0.82999433924766</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B59" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C59" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="D59" s="5" t="s">
-        <v>9</v>
+        <v>5</v>
+      </c>
+      <c r="C59" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D59" s="1" t="s">
+        <v>8</v>
       </c>
       <c r="E59" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.745980665929878</v>
+        <v>0.0394516592915679</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1310,15 +1262,15 @@
       <c r="B60" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C60" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="D60" s="5" t="s">
-        <v>9</v>
+      <c r="C60" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D60" s="1" t="s">
+        <v>8</v>
       </c>
       <c r="E60" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.280773708810783</v>
+        <v>0.194328067123851</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1328,89 +1280,89 @@
       <c r="B61" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C61" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="D61" s="5" t="s">
-        <v>9</v>
+      <c r="C61" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D61" s="1" t="s">
+        <v>8</v>
       </c>
       <c r="E61" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.61703701506609</v>
+        <v>0.228476942232872</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="2"/>
       <c r="B62" s="2"/>
-      <c r="C62" s="6"/>
+      <c r="C62" s="4"/>
     </row>
     <row r="63" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="2"/>
-      <c r="B63" s="6"/>
+      <c r="B63" s="4"/>
     </row>
     <row r="64" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="2"/>
-      <c r="B64" s="6"/>
+      <c r="B64" s="4"/>
     </row>
     <row r="65" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="2"/>
-      <c r="B65" s="6"/>
+      <c r="B65" s="4"/>
     </row>
     <row r="66" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A66" s="6"/>
+      <c r="A66" s="4"/>
       <c r="B66" s="2"/>
     </row>
     <row r="67" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A67" s="6"/>
+      <c r="A67" s="4"/>
       <c r="B67" s="2"/>
     </row>
     <row r="68" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A68" s="6"/>
+      <c r="A68" s="4"/>
       <c r="B68" s="2"/>
     </row>
     <row r="69" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="2"/>
-      <c r="B69" s="6"/>
+      <c r="B69" s="4"/>
     </row>
     <row r="70" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="2"/>
-      <c r="B70" s="6"/>
+      <c r="B70" s="4"/>
     </row>
     <row r="71" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A71" s="6"/>
+      <c r="A71" s="4"/>
       <c r="B71" s="2"/>
     </row>
     <row r="72" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="2"/>
-      <c r="B72" s="6"/>
+      <c r="B72" s="4"/>
     </row>
     <row r="73" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A73" s="6"/>
+      <c r="A73" s="4"/>
       <c r="B73" s="2"/>
     </row>
     <row r="74" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A74" s="6"/>
+      <c r="A74" s="4"/>
       <c r="B74" s="2"/>
     </row>
     <row r="75" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="2"/>
-      <c r="B75" s="6"/>
+      <c r="B75" s="4"/>
     </row>
     <row r="76" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="2"/>
-      <c r="B76" s="6"/>
+      <c r="B76" s="4"/>
     </row>
     <row r="77" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A77" s="6"/>
+      <c r="A77" s="4"/>
       <c r="B77" s="2"/>
     </row>
     <row r="78" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A78" s="6"/>
+      <c r="A78" s="4"/>
       <c r="B78" s="2"/>
     </row>
     <row r="79" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A79" s="2"/>
-      <c r="B79" s="6"/>
+      <c r="B79" s="4"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>

<commit_message>
committing edits on timing of start wall lowering and some modification  of the single T maze code
</commit_message>
<xml_diff>
--- a/src/omniroute_operation/src/single_T_maze/Training_Trials .xlsx
+++ b/src/omniroute_operation/src/single_T_maze/Training_Trials .xlsx
@@ -59,7 +59,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="8">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -94,6 +94,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
@@ -145,7 +151,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -163,6 +169,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -185,11 +195,11 @@
   </sheetPr>
   <dimension ref="A1:E79"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A28" colorId="64" zoomScale="250" zoomScaleNormal="250" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G55" activeCellId="0" sqref="G55"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="250" zoomScaleNormal="250" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G19" activeCellId="0" sqref="G19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.875" defaultRowHeight="13" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.89453125" defaultRowHeight="13" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="5" min="5" style="0" width="11.71"/>
   </cols>
@@ -226,7 +236,7 @@
       </c>
       <c r="E2" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.325341825288847</v>
+        <v>0.139056621473216</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -244,7 +254,7 @@
       </c>
       <c r="E3" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.736949194848838</v>
+        <v>0.367999111831412</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -262,7 +272,7 @@
       </c>
       <c r="E4" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.76950926060755</v>
+        <v>0.652607538652187</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -280,7 +290,7 @@
       </c>
       <c r="E5" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.198476696039102</v>
+        <v>0.0966056782205884</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -298,7 +308,7 @@
       </c>
       <c r="E6" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.572876886956201</v>
+        <v>0.376157388817091</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -316,7 +326,7 @@
       </c>
       <c r="E7" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.14124046393787</v>
+        <v>0.363530619376528</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -334,15 +344,15 @@
       </c>
       <c r="E8" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.349876633085204</v>
+        <v>0.443259490775759</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C9" s="3" t="s">
         <v>7</v>
@@ -352,15 +362,15 @@
       </c>
       <c r="E9" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.859936170081302</v>
+        <v>0.212131354220057</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C10" s="3" t="s">
         <v>7</v>
@@ -370,7 +380,7 @@
       </c>
       <c r="E10" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.0333754070501721</v>
+        <v>0.322251663596433</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -388,7 +398,7 @@
       </c>
       <c r="E11" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.210536406038008</v>
+        <v>0.883945171288113</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -406,7 +416,7 @@
       </c>
       <c r="E12" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.817265043890606</v>
+        <v>0.505929464010691</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -424,12 +434,12 @@
       </c>
       <c r="E13" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.285758522491754</v>
+        <v>0.001339741919158</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="2" t="s">
-        <v>5</v>
+      <c r="A14" s="4" t="s">
+        <v>6</v>
       </c>
       <c r="B14" s="2" t="s">
         <v>5</v>
@@ -442,7 +452,7 @@
       </c>
       <c r="E14" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.0380000034580211</v>
+        <v>0.640533841167754</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -460,7 +470,7 @@
       </c>
       <c r="E15" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.906227525004015</v>
+        <v>0.982043294481426</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -478,7 +488,7 @@
       </c>
       <c r="E16" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.32416219018021</v>
+        <v>0.865874576437069</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -496,7 +506,7 @@
       </c>
       <c r="E17" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.805858717578101</v>
+        <v>0.980421099317531</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -514,7 +524,7 @@
       </c>
       <c r="E18" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.561488343663837</v>
+        <v>0.897173860704208</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -532,7 +542,7 @@
       </c>
       <c r="E19" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.210259245844799</v>
+        <v>0.570702206174095</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -550,7 +560,7 @@
       </c>
       <c r="E20" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.715537780200506</v>
+        <v>0.481166786294398</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -568,7 +578,7 @@
       </c>
       <c r="E21" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.679905647113464</v>
+        <v>0.0484605097353762</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -586,7 +596,7 @@
       </c>
       <c r="E22" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.705341658699668</v>
+        <v>0.467992700640346</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -604,7 +614,7 @@
       </c>
       <c r="E23" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.900037112859407</v>
+        <v>0.902449649552502</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -622,7 +632,7 @@
       </c>
       <c r="E24" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.738065161912534</v>
+        <v>0.450497301287591</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -640,14 +650,14 @@
       </c>
       <c r="E25" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.298767366707625</v>
+        <v>0.120230117608668</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="B26" s="2" t="s">
+      <c r="A26" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B26" s="4" t="s">
         <v>6</v>
       </c>
       <c r="C26" s="3" t="s">
@@ -658,7 +668,7 @@
       </c>
       <c r="E26" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.0248798426137125</v>
+        <v>0.787552079517133</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -676,7 +686,7 @@
       </c>
       <c r="E27" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.361025096301436</v>
+        <v>0.828843220003298</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -694,7 +704,7 @@
       </c>
       <c r="E28" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.463477879596986</v>
+        <v>0.0289597410852436</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -712,7 +722,7 @@
       </c>
       <c r="E29" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.899677576848432</v>
+        <v>0.41792899646065</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -730,7 +740,7 @@
       </c>
       <c r="E30" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.17486489363463</v>
+        <v>0.713278646029349</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -748,7 +758,7 @@
       </c>
       <c r="E31" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.919198393139249</v>
+        <v>0.495389267735773</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -758,7 +768,7 @@
       <c r="B32" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C32" s="4" t="s">
+      <c r="C32" s="5" t="s">
         <v>9</v>
       </c>
       <c r="D32" s="1" t="s">
@@ -766,7 +776,7 @@
       </c>
       <c r="E32" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.932599751045215</v>
+        <v>0.176469177679815</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -776,7 +786,7 @@
       <c r="B33" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C33" s="4" t="s">
+      <c r="C33" s="5" t="s">
         <v>9</v>
       </c>
       <c r="D33" s="1" t="s">
@@ -784,7 +794,7 @@
       </c>
       <c r="E33" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.687349431227975</v>
+        <v>0.956581905037498</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -794,7 +804,7 @@
       <c r="B34" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C34" s="4" t="s">
+      <c r="C34" s="5" t="s">
         <v>9</v>
       </c>
       <c r="D34" s="1" t="s">
@@ -802,7 +812,7 @@
       </c>
       <c r="E34" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.668866102360497</v>
+        <v>0.995059798325736</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -812,7 +822,7 @@
       <c r="B35" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C35" s="4" t="s">
+      <c r="C35" s="5" t="s">
         <v>9</v>
       </c>
       <c r="D35" s="1" t="s">
@@ -820,7 +830,7 @@
       </c>
       <c r="E35" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.299113711228443</v>
+        <v>0.388185140484684</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -830,7 +840,7 @@
       <c r="B36" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C36" s="4" t="s">
+      <c r="C36" s="5" t="s">
         <v>9</v>
       </c>
       <c r="D36" s="1" t="s">
@@ -838,7 +848,7 @@
       </c>
       <c r="E36" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.253136182277389</v>
+        <v>0.133599515698617</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -848,7 +858,7 @@
       <c r="B37" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C37" s="4" t="s">
+      <c r="C37" s="5" t="s">
         <v>9</v>
       </c>
       <c r="D37" s="1" t="s">
@@ -856,7 +866,7 @@
       </c>
       <c r="E37" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.978108447662928</v>
+        <v>0.603238972777347</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -866,7 +876,7 @@
       <c r="B38" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C38" s="4" t="s">
+      <c r="C38" s="5" t="s">
         <v>9</v>
       </c>
       <c r="D38" s="1" t="s">
@@ -874,7 +884,7 @@
       </c>
       <c r="E38" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.350758258224709</v>
+        <v>0.547202351547818</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -884,7 +894,7 @@
       <c r="B39" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C39" s="4" t="s">
+      <c r="C39" s="5" t="s">
         <v>9</v>
       </c>
       <c r="D39" s="1" t="s">
@@ -892,7 +902,7 @@
       </c>
       <c r="E39" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.530027475603528</v>
+        <v>0.172346479680367</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -902,7 +912,7 @@
       <c r="B40" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C40" s="4" t="s">
+      <c r="C40" s="5" t="s">
         <v>9</v>
       </c>
       <c r="D40" s="1" t="s">
@@ -910,7 +920,7 @@
       </c>
       <c r="E40" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.0932446401893503</v>
+        <v>0.5393019590832</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -920,7 +930,7 @@
       <c r="B41" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C41" s="4" t="s">
+      <c r="C41" s="5" t="s">
         <v>9</v>
       </c>
       <c r="D41" s="1" t="s">
@@ -928,7 +938,7 @@
       </c>
       <c r="E41" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.00586027250121808</v>
+        <v>0.299909620131257</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -938,7 +948,7 @@
       <c r="B42" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C42" s="4" t="s">
+      <c r="C42" s="5" t="s">
         <v>9</v>
       </c>
       <c r="D42" s="1" t="s">
@@ -946,7 +956,7 @@
       </c>
       <c r="E42" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.134216457692807</v>
+        <v>0.695658796492837</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -956,7 +966,7 @@
       <c r="B43" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C43" s="4" t="s">
+      <c r="C43" s="5" t="s">
         <v>9</v>
       </c>
       <c r="D43" s="1" t="s">
@@ -964,7 +974,7 @@
       </c>
       <c r="E43" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.807968323442944</v>
+        <v>0.996978848218224</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -974,7 +984,7 @@
       <c r="B44" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C44" s="4" t="s">
+      <c r="C44" s="5" t="s">
         <v>9</v>
       </c>
       <c r="D44" s="1" t="s">
@@ -982,7 +992,7 @@
       </c>
       <c r="E44" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.867169010774887</v>
+        <v>0.844640629073256</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -992,7 +1002,7 @@
       <c r="B45" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C45" s="4" t="s">
+      <c r="C45" s="5" t="s">
         <v>9</v>
       </c>
       <c r="D45" s="1" t="s">
@@ -1000,7 +1010,7 @@
       </c>
       <c r="E45" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.736377004438553</v>
+        <v>0.716399247629953</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1010,7 +1020,7 @@
       <c r="B46" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C46" s="4" t="s">
+      <c r="C46" s="5" t="s">
         <v>9</v>
       </c>
       <c r="D46" s="1" t="s">
@@ -1018,7 +1028,7 @@
       </c>
       <c r="E46" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.0754379602488955</v>
+        <v>0.359470697094932</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1028,7 +1038,7 @@
       <c r="B47" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C47" s="4" t="s">
+      <c r="C47" s="5" t="s">
         <v>9</v>
       </c>
       <c r="D47" s="1" t="s">
@@ -1036,7 +1046,7 @@
       </c>
       <c r="E47" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.650459452788075</v>
+        <v>0.127945257221961</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1046,7 +1056,7 @@
       <c r="B48" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C48" s="4" t="s">
+      <c r="C48" s="5" t="s">
         <v>9</v>
       </c>
       <c r="D48" s="1" t="s">
@@ -1054,7 +1064,7 @@
       </c>
       <c r="E48" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.907833678001237</v>
+        <v>0.317706367636135</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1064,7 +1074,7 @@
       <c r="B49" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C49" s="4" t="s">
+      <c r="C49" s="5" t="s">
         <v>9</v>
       </c>
       <c r="D49" s="1" t="s">
@@ -1072,7 +1082,7 @@
       </c>
       <c r="E49" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.885722060330212</v>
+        <v>0.172454735315456</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1082,7 +1092,7 @@
       <c r="B50" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C50" s="4" t="s">
+      <c r="C50" s="5" t="s">
         <v>9</v>
       </c>
       <c r="D50" s="1" t="s">
@@ -1090,7 +1100,7 @@
       </c>
       <c r="E50" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.78925459966701</v>
+        <v>0.206308701667511</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1100,7 +1110,7 @@
       <c r="B51" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C51" s="4" t="s">
+      <c r="C51" s="5" t="s">
         <v>9</v>
       </c>
       <c r="D51" s="1" t="s">
@@ -1108,7 +1118,7 @@
       </c>
       <c r="E51" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.582980643174923</v>
+        <v>0.12159785343824</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1118,7 +1128,7 @@
       <c r="B52" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C52" s="4" t="s">
+      <c r="C52" s="5" t="s">
         <v>9</v>
       </c>
       <c r="D52" s="1" t="s">
@@ -1126,7 +1136,7 @@
       </c>
       <c r="E52" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.992398338876803</v>
+        <v>0.168154951491064</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1136,7 +1146,7 @@
       <c r="B53" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C53" s="4" t="s">
+      <c r="C53" s="5" t="s">
         <v>9</v>
       </c>
       <c r="D53" s="1" t="s">
@@ -1144,7 +1154,7 @@
       </c>
       <c r="E53" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.224072444476191</v>
+        <v>0.529227904252339</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1154,7 +1164,7 @@
       <c r="B54" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C54" s="4" t="s">
+      <c r="C54" s="5" t="s">
         <v>9</v>
       </c>
       <c r="D54" s="1" t="s">
@@ -1162,7 +1172,7 @@
       </c>
       <c r="E54" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.483531593234427</v>
+        <v>0.777202597010036</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1172,7 +1182,7 @@
       <c r="B55" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C55" s="4" t="s">
+      <c r="C55" s="5" t="s">
         <v>9</v>
       </c>
       <c r="D55" s="1" t="s">
@@ -1180,7 +1190,7 @@
       </c>
       <c r="E55" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.670818653005099</v>
+        <v>0.00542497859233546</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1190,7 +1200,7 @@
       <c r="B56" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C56" s="4" t="s">
+      <c r="C56" s="5" t="s">
         <v>9</v>
       </c>
       <c r="D56" s="1" t="s">
@@ -1198,7 +1208,7 @@
       </c>
       <c r="E56" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.862101870153993</v>
+        <v>0.735083289792967</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1208,7 +1218,7 @@
       <c r="B57" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C57" s="4" t="s">
+      <c r="C57" s="5" t="s">
         <v>9</v>
       </c>
       <c r="D57" s="1" t="s">
@@ -1216,7 +1226,7 @@
       </c>
       <c r="E57" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.289151210477785</v>
+        <v>0.586470705897012</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1226,7 +1236,7 @@
       <c r="B58" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C58" s="4" t="s">
+      <c r="C58" s="5" t="s">
         <v>9</v>
       </c>
       <c r="D58" s="1" t="s">
@@ -1234,7 +1244,7 @@
       </c>
       <c r="E58" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.82999433924766</v>
+        <v>0.01719203598452</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1244,7 +1254,7 @@
       <c r="B59" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C59" s="4" t="s">
+      <c r="C59" s="5" t="s">
         <v>9</v>
       </c>
       <c r="D59" s="1" t="s">
@@ -1252,7 +1262,7 @@
       </c>
       <c r="E59" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.0394516592915679</v>
+        <v>0.963268089721598</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1262,7 +1272,7 @@
       <c r="B60" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C60" s="4" t="s">
+      <c r="C60" s="5" t="s">
         <v>9</v>
       </c>
       <c r="D60" s="1" t="s">
@@ -1270,7 +1280,7 @@
       </c>
       <c r="E60" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.194328067123851</v>
+        <v>0.164965220955052</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1280,7 +1290,7 @@
       <c r="B61" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C61" s="4" t="s">
+      <c r="C61" s="5" t="s">
         <v>9</v>
       </c>
       <c r="D61" s="1" t="s">
@@ -1288,81 +1298,81 @@
       </c>
       <c r="E61" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.228476942232872</v>
+        <v>0.59644432131352</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="2"/>
       <c r="B62" s="2"/>
-      <c r="C62" s="4"/>
+      <c r="C62" s="5"/>
     </row>
     <row r="63" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="2"/>
-      <c r="B63" s="4"/>
+      <c r="B63" s="5"/>
     </row>
     <row r="64" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="2"/>
-      <c r="B64" s="4"/>
+      <c r="B64" s="5"/>
     </row>
     <row r="65" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="2"/>
-      <c r="B65" s="4"/>
+      <c r="B65" s="5"/>
     </row>
     <row r="66" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A66" s="4"/>
+      <c r="A66" s="5"/>
       <c r="B66" s="2"/>
     </row>
     <row r="67" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A67" s="4"/>
+      <c r="A67" s="5"/>
       <c r="B67" s="2"/>
     </row>
     <row r="68" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A68" s="4"/>
+      <c r="A68" s="5"/>
       <c r="B68" s="2"/>
     </row>
     <row r="69" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="2"/>
-      <c r="B69" s="4"/>
+      <c r="B69" s="5"/>
     </row>
     <row r="70" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="2"/>
-      <c r="B70" s="4"/>
+      <c r="B70" s="5"/>
     </row>
     <row r="71" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A71" s="4"/>
+      <c r="A71" s="5"/>
       <c r="B71" s="2"/>
     </row>
     <row r="72" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="2"/>
-      <c r="B72" s="4"/>
+      <c r="B72" s="5"/>
     </row>
     <row r="73" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A73" s="4"/>
+      <c r="A73" s="5"/>
       <c r="B73" s="2"/>
     </row>
     <row r="74" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A74" s="4"/>
+      <c r="A74" s="5"/>
       <c r="B74" s="2"/>
     </row>
     <row r="75" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="2"/>
-      <c r="B75" s="4"/>
+      <c r="B75" s="5"/>
     </row>
     <row r="76" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="2"/>
-      <c r="B76" s="4"/>
+      <c r="B76" s="5"/>
     </row>
     <row r="77" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A77" s="4"/>
+      <c r="A77" s="5"/>
       <c r="B77" s="2"/>
     </row>
     <row r="78" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A78" s="4"/>
+      <c r="A78" s="5"/>
       <c r="B78" s="2"/>
     </row>
     <row r="79" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A79" s="2"/>
-      <c r="B79" s="4"/>
+      <c r="B79" s="5"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>

<commit_message>
adding delays to nodes initiating
</commit_message>
<xml_diff>
--- a/src/omniroute_operation/src/single_T_maze/Training_Trials .xlsx
+++ b/src/omniroute_operation/src/single_T_maze/Training_Trials .xlsx
@@ -43,13 +43,13 @@
     <t xml:space="preserve">Triangle</t>
   </si>
   <si>
-    <t xml:space="preserve">Green</t>
+    <t xml:space="preserve">Black</t>
   </si>
   <si>
     <t xml:space="preserve">forced_choice</t>
   </si>
   <si>
-    <t xml:space="preserve">Black</t>
+    <t xml:space="preserve">Green</t>
   </si>
 </sst>
 </file>
@@ -59,7 +59,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="8">
+  <fonts count="7">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -89,7 +89,7 @@
       <charset val="1"/>
     </font>
     <font>
-      <sz val="10"/>
+      <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -97,12 +97,6 @@
     </font>
     <font>
       <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -151,7 +145,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -172,10 +166,6 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -193,13 +183,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E79"/>
+  <dimension ref="A1:G109"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="250" zoomScaleNormal="250" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G19" activeCellId="0" sqref="G19"/>
+      <selection pane="topLeft" activeCell="G23" activeCellId="0" sqref="G23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.89453125" defaultRowHeight="13" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.9140625" defaultRowHeight="13" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="5" min="5" style="0" width="11.71"/>
   </cols>
@@ -221,7 +211,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="s">
         <v>5</v>
       </c>
@@ -236,10 +226,10 @@
       </c>
       <c r="E2" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.139056621473216</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>0.201596252114478</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="2" t="s">
         <v>5</v>
       </c>
@@ -254,15 +244,15 @@
       </c>
       <c r="E3" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.367999111831412</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>0.854573417295986</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C4" s="3" t="s">
         <v>7</v>
@@ -272,10 +262,10 @@
       </c>
       <c r="E4" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.652607538652187</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>0.108485288459586</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="2" t="s">
         <v>6</v>
       </c>
@@ -290,15 +280,15 @@
       </c>
       <c r="E5" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.0966056782205884</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>0.479683295977589</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C6" s="3" t="s">
         <v>7</v>
@@ -308,15 +298,15 @@
       </c>
       <c r="E6" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.376157388817091</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>0.762729310753049</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C7" s="3" t="s">
         <v>7</v>
@@ -326,15 +316,15 @@
       </c>
       <c r="E7" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.363530619376528</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>0.561546080931723</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C8" s="3" t="s">
         <v>7</v>
@@ -344,15 +334,15 @@
       </c>
       <c r="E8" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.443259490775759</v>
-      </c>
-    </row>
-    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>0.716324886058473</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C9" s="3" t="s">
         <v>7</v>
@@ -362,15 +352,15 @@
       </c>
       <c r="E9" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.212131354220057</v>
-      </c>
-    </row>
-    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>0.624007690950124</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C10" s="3" t="s">
         <v>7</v>
@@ -380,15 +370,15 @@
       </c>
       <c r="E10" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.322251663596433</v>
-      </c>
-    </row>
-    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>0.274395860989766</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C11" s="3" t="s">
         <v>7</v>
@@ -398,10 +388,10 @@
       </c>
       <c r="E11" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.883945171288113</v>
-      </c>
-    </row>
-    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>0.563315983448688</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="2" t="s">
         <v>6</v>
       </c>
@@ -416,10 +406,10 @@
       </c>
       <c r="E12" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.505929464010691</v>
-      </c>
-    </row>
-    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>0.211451302285842</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="2" t="s">
         <v>5</v>
       </c>
@@ -434,15 +424,15 @@
       </c>
       <c r="E13" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.001339741919158</v>
-      </c>
-    </row>
-    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="4" t="s">
-        <v>6</v>
+        <v>0.234529178191358</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="2" t="s">
+        <v>5</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C14" s="3" t="s">
         <v>7</v>
@@ -452,10 +442,10 @@
       </c>
       <c r="E14" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.640533841167754</v>
-      </c>
-    </row>
-    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>0.342252982687629</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="2" t="s">
         <v>6</v>
       </c>
@@ -470,15 +460,15 @@
       </c>
       <c r="E15" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.982043294481426</v>
-      </c>
-    </row>
-    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>0.32195248647352</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C16" s="3" t="s">
         <v>7</v>
@@ -488,15 +478,15 @@
       </c>
       <c r="E16" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.865874576437069</v>
-      </c>
-    </row>
-    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>0.0460558498803287</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C17" s="3" t="s">
         <v>7</v>
@@ -506,15 +496,15 @@
       </c>
       <c r="E17" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.980421099317531</v>
-      </c>
-    </row>
-    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>0.525923079162625</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C18" s="3" t="s">
         <v>7</v>
@@ -524,15 +514,15 @@
       </c>
       <c r="E18" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.897173860704208</v>
-      </c>
-    </row>
-    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>0.191403950643939</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C19" s="3" t="s">
         <v>7</v>
@@ -542,10 +532,10 @@
       </c>
       <c r="E19" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.570702206174095</v>
-      </c>
-    </row>
-    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>0.364730394325668</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="2" t="s">
         <v>6</v>
       </c>
@@ -560,10 +550,10 @@
       </c>
       <c r="E20" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.481166786294398</v>
-      </c>
-    </row>
-    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>0.191904782580312</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="2" t="s">
         <v>5</v>
       </c>
@@ -578,10 +568,10 @@
       </c>
       <c r="E21" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.0484605097353762</v>
-      </c>
-    </row>
-    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>0.755471983097356</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="2" t="s">
         <v>6</v>
       </c>
@@ -596,15 +586,15 @@
       </c>
       <c r="E22" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.467992700640346</v>
-      </c>
-    </row>
-    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>0.519295617900995</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C23" s="3" t="s">
         <v>7</v>
@@ -614,15 +604,15 @@
       </c>
       <c r="E23" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.902449649552502</v>
-      </c>
-    </row>
-    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>0.43762649646653</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C24" s="3" t="s">
         <v>7</v>
@@ -632,15 +622,15 @@
       </c>
       <c r="E24" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.450497301287591</v>
-      </c>
-    </row>
-    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>0.385175725141759</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C25" s="3" t="s">
         <v>7</v>
@@ -650,15 +640,15 @@
       </c>
       <c r="E25" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.120230117608668</v>
-      </c>
-    </row>
-    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="B26" s="4" t="s">
-        <v>6</v>
+        <v>0.167022404887932</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>5</v>
       </c>
       <c r="C26" s="3" t="s">
         <v>7</v>
@@ -668,10 +658,10 @@
       </c>
       <c r="E26" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.787552079517133</v>
-      </c>
-    </row>
-    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>0.961851221048138</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="2" t="s">
         <v>5</v>
       </c>
@@ -686,10 +676,10 @@
       </c>
       <c r="E27" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.828843220003298</v>
-      </c>
-    </row>
-    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>0.107907032588013</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="2" t="s">
         <v>6</v>
       </c>
@@ -704,15 +694,15 @@
       </c>
       <c r="E28" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.0289597410852436</v>
-      </c>
-    </row>
-    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>0.562962234199314</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C29" s="3" t="s">
         <v>7</v>
@@ -722,10 +712,10 @@
       </c>
       <c r="E29" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.41792899646065</v>
-      </c>
-    </row>
-    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>0.161828181400239</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="2" t="s">
         <v>5</v>
       </c>
@@ -740,10 +730,10 @@
       </c>
       <c r="E30" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.713278646029349</v>
-      </c>
-    </row>
-    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>0.363409189024345</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="2" t="s">
         <v>6</v>
       </c>
@@ -758,17 +748,17 @@
       </c>
       <c r="E31" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.495389267735773</v>
-      </c>
-    </row>
-    <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>0.547864413932919</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="2" t="s">
         <v>5</v>
       </c>
       <c r="B32" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C32" s="5" t="s">
+      <c r="C32" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D32" s="1" t="s">
@@ -776,17 +766,17 @@
       </c>
       <c r="E32" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.176469177679815</v>
-      </c>
-    </row>
-    <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>0.463057586320547</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="2" t="s">
         <v>5</v>
       </c>
       <c r="B33" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C33" s="5" t="s">
+      <c r="C33" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D33" s="1" t="s">
@@ -794,17 +784,17 @@
       </c>
       <c r="E33" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.956581905037498</v>
-      </c>
-    </row>
-    <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>0.00858714055749718</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C34" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C34" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D34" s="1" t="s">
@@ -812,17 +802,17 @@
       </c>
       <c r="E34" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.995059798325736</v>
-      </c>
-    </row>
-    <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>0.151722993684865</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="2" t="s">
         <v>6</v>
       </c>
       <c r="B35" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C35" s="5" t="s">
+      <c r="C35" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D35" s="1" t="s">
@@ -830,17 +820,17 @@
       </c>
       <c r="E35" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.388185140484684</v>
-      </c>
-    </row>
-    <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>0.434301287991968</v>
+      </c>
+    </row>
+    <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C36" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C36" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D36" s="1" t="s">
@@ -848,17 +838,17 @@
       </c>
       <c r="E36" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.133599515698617</v>
-      </c>
-    </row>
-    <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>0.469990863124009</v>
+      </c>
+    </row>
+    <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C37" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C37" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D37" s="1" t="s">
@@ -866,17 +856,17 @@
       </c>
       <c r="E37" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.603238972777347</v>
-      </c>
-    </row>
-    <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>0.62954034487347</v>
+      </c>
+    </row>
+    <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C38" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C38" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D38" s="1" t="s">
@@ -884,17 +874,17 @@
       </c>
       <c r="E38" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.547202351547818</v>
-      </c>
-    </row>
-    <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>0.452593420839222</v>
+      </c>
+    </row>
+    <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C39" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C39" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D39" s="1" t="s">
@@ -902,17 +892,17 @@
       </c>
       <c r="E39" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.172346479680367</v>
-      </c>
-    </row>
-    <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>0.427122572506873</v>
+      </c>
+    </row>
+    <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C40" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C40" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D40" s="1" t="s">
@@ -920,17 +910,17 @@
       </c>
       <c r="E40" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.5393019590832</v>
-      </c>
-    </row>
-    <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>0.451885980339873</v>
+      </c>
+    </row>
+    <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C41" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C41" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D41" s="1" t="s">
@@ -938,17 +928,17 @@
       </c>
       <c r="E41" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.299909620131257</v>
-      </c>
-    </row>
-    <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>0.241566567665257</v>
+      </c>
+    </row>
+    <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="2" t="s">
         <v>6</v>
       </c>
       <c r="B42" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C42" s="5" t="s">
+      <c r="C42" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D42" s="1" t="s">
@@ -956,17 +946,17 @@
       </c>
       <c r="E42" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.695658796492837</v>
-      </c>
-    </row>
-    <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>0.0873617022954323</v>
+      </c>
+    </row>
+    <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="2" t="s">
         <v>5</v>
       </c>
       <c r="B43" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C43" s="5" t="s">
+      <c r="C43" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D43" s="1" t="s">
@@ -974,17 +964,17 @@
       </c>
       <c r="E43" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.996978848218224</v>
-      </c>
-    </row>
-    <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>0.654745678762566</v>
+      </c>
+    </row>
+    <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C44" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C44" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D44" s="1" t="s">
@@ -992,17 +982,17 @@
       </c>
       <c r="E44" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.844640629073256</v>
-      </c>
-    </row>
-    <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>0.235453647892564</v>
+      </c>
+    </row>
+    <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="2" t="s">
         <v>6</v>
       </c>
       <c r="B45" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C45" s="5" t="s">
+      <c r="C45" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D45" s="1" t="s">
@@ -1010,17 +1000,17 @@
       </c>
       <c r="E45" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.716399247629953</v>
-      </c>
-    </row>
-    <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>0.177147831379464</v>
+      </c>
+    </row>
+    <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C46" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C46" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D46" s="1" t="s">
@@ -1028,17 +1018,17 @@
       </c>
       <c r="E46" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.359470697094932</v>
-      </c>
-    </row>
-    <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>0.388145458854212</v>
+      </c>
+    </row>
+    <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C47" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C47" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D47" s="1" t="s">
@@ -1046,17 +1036,17 @@
       </c>
       <c r="E47" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.127945257221961</v>
-      </c>
-    </row>
-    <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>0.680976263032193</v>
+      </c>
+    </row>
+    <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C48" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C48" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D48" s="1" t="s">
@@ -1064,17 +1054,17 @@
       </c>
       <c r="E48" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.317706367636135</v>
-      </c>
-    </row>
-    <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>0.303791905376572</v>
+      </c>
+    </row>
+    <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C49" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C49" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D49" s="1" t="s">
@@ -1082,17 +1072,17 @@
       </c>
       <c r="E49" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.172454735315456</v>
-      </c>
-    </row>
-    <row r="50" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>0.765956168588507</v>
+      </c>
+    </row>
+    <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="2" t="s">
         <v>6</v>
       </c>
       <c r="B50" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C50" s="5" t="s">
+      <c r="C50" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D50" s="1" t="s">
@@ -1100,17 +1090,17 @@
       </c>
       <c r="E50" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.206308701667511</v>
-      </c>
-    </row>
-    <row r="51" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>0.764106977949451</v>
+      </c>
+    </row>
+    <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="2" t="s">
         <v>5</v>
       </c>
       <c r="B51" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C51" s="5" t="s">
+      <c r="C51" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D51" s="1" t="s">
@@ -1118,17 +1108,17 @@
       </c>
       <c r="E51" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.12159785343824</v>
-      </c>
-    </row>
-    <row r="52" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>0.402000417038944</v>
+      </c>
+    </row>
+    <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="2" t="s">
         <v>6</v>
       </c>
       <c r="B52" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C52" s="5" t="s">
+      <c r="C52" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D52" s="1" t="s">
@@ -1136,17 +1126,17 @@
       </c>
       <c r="E52" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.168154951491064</v>
-      </c>
-    </row>
-    <row r="53" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>0.566533431321613</v>
+      </c>
+    </row>
+    <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B53" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C53" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C53" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D53" s="1" t="s">
@@ -1154,17 +1144,17 @@
       </c>
       <c r="E53" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.529227904252339</v>
-      </c>
-    </row>
-    <row r="54" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>0.4318043548909</v>
+      </c>
+    </row>
+    <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C54" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C54" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D54" s="1" t="s">
@@ -1172,17 +1162,17 @@
       </c>
       <c r="E54" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.777202597010036</v>
-      </c>
-    </row>
-    <row r="55" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>0.407923340946041</v>
+      </c>
+    </row>
+    <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C55" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C55" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D55" s="1" t="s">
@@ -1190,17 +1180,17 @@
       </c>
       <c r="E55" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.00542497859233546</v>
-      </c>
-    </row>
-    <row r="56" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>0.569627604921605</v>
+      </c>
+    </row>
+    <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="2" t="s">
         <v>6</v>
       </c>
       <c r="B56" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C56" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C56" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D56" s="1" t="s">
@@ -1208,17 +1198,17 @@
       </c>
       <c r="E56" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.735083289792967</v>
-      </c>
-    </row>
-    <row r="57" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>0.252003581977478</v>
+      </c>
+    </row>
+    <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="2" t="s">
         <v>5</v>
       </c>
       <c r="B57" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C57" s="5" t="s">
+      <c r="C57" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D57" s="1" t="s">
@@ -1226,17 +1216,17 @@
       </c>
       <c r="E57" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.586470705897012</v>
-      </c>
-    </row>
-    <row r="58" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>0.735945499172982</v>
+      </c>
+    </row>
+    <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="2" t="s">
         <v>6</v>
       </c>
       <c r="B58" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C58" s="5" t="s">
+      <c r="C58" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D58" s="1" t="s">
@@ -1244,17 +1234,17 @@
       </c>
       <c r="E58" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.01719203598452</v>
-      </c>
-    </row>
-    <row r="59" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>0.209121632742129</v>
+      </c>
+    </row>
+    <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B59" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C59" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C59" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D59" s="1" t="s">
@@ -1262,17 +1252,17 @@
       </c>
       <c r="E59" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.963268089721598</v>
-      </c>
-    </row>
-    <row r="60" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>0.290018465757379</v>
+      </c>
+    </row>
+    <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="2" t="s">
         <v>5</v>
       </c>
       <c r="B60" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C60" s="5" t="s">
+      <c r="C60" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D60" s="1" t="s">
@@ -1280,17 +1270,17 @@
       </c>
       <c r="E60" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.164965220955052</v>
-      </c>
-    </row>
-    <row r="61" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>0.243266235400438</v>
+      </c>
+    </row>
+    <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="2" t="s">
         <v>6</v>
       </c>
       <c r="B61" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C61" s="5" t="s">
+      <c r="C61" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D61" s="1" t="s">
@@ -1298,81 +1288,440 @@
       </c>
       <c r="E61" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.59644432131352</v>
-      </c>
-    </row>
-    <row r="62" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>0.979079881506249</v>
+      </c>
+    </row>
+    <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="2"/>
       <c r="B62" s="2"/>
-      <c r="C62" s="5"/>
-    </row>
-    <row r="63" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C62" s="4"/>
+      <c r="D62" s="1"/>
+      <c r="E62" s="2"/>
+      <c r="F62" s="2"/>
+      <c r="G62" s="4"/>
+    </row>
+    <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="2"/>
-      <c r="B63" s="5"/>
-    </row>
-    <row r="64" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B63" s="2"/>
+      <c r="C63" s="4"/>
+      <c r="D63" s="1"/>
+      <c r="E63" s="2"/>
+      <c r="F63" s="2"/>
+      <c r="G63" s="4"/>
+    </row>
+    <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="2"/>
-      <c r="B64" s="5"/>
-    </row>
-    <row r="65" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B64" s="2"/>
+      <c r="C64" s="4"/>
+      <c r="D64" s="1"/>
+      <c r="E64" s="2"/>
+      <c r="F64" s="2"/>
+      <c r="G64" s="4"/>
+    </row>
+    <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="2"/>
-      <c r="B65" s="5"/>
-    </row>
-    <row r="66" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A66" s="5"/>
+      <c r="B65" s="2"/>
+      <c r="C65" s="4"/>
+      <c r="D65" s="1"/>
+      <c r="E65" s="2"/>
+      <c r="F65" s="2"/>
+      <c r="G65" s="4"/>
+    </row>
+    <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A66" s="2"/>
       <c r="B66" s="2"/>
-    </row>
-    <row r="67" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A67" s="5"/>
+      <c r="C66" s="4"/>
+      <c r="D66" s="1"/>
+      <c r="E66" s="2"/>
+      <c r="F66" s="2"/>
+      <c r="G66" s="4"/>
+    </row>
+    <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A67" s="2"/>
       <c r="B67" s="2"/>
-    </row>
-    <row r="68" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A68" s="5"/>
+      <c r="C67" s="4"/>
+      <c r="D67" s="1"/>
+      <c r="E67" s="2"/>
+      <c r="F67" s="2"/>
+      <c r="G67" s="4"/>
+    </row>
+    <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A68" s="2"/>
       <c r="B68" s="2"/>
-    </row>
-    <row r="69" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C68" s="4"/>
+      <c r="D68" s="1"/>
+      <c r="E68" s="2"/>
+      <c r="F68" s="2"/>
+      <c r="G68" s="4"/>
+    </row>
+    <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="2"/>
-      <c r="B69" s="5"/>
-    </row>
-    <row r="70" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B69" s="2"/>
+      <c r="C69" s="4"/>
+      <c r="D69" s="1"/>
+      <c r="E69" s="2"/>
+      <c r="F69" s="2"/>
+      <c r="G69" s="4"/>
+    </row>
+    <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="2"/>
-      <c r="B70" s="5"/>
-    </row>
-    <row r="71" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A71" s="5"/>
+      <c r="B70" s="2"/>
+      <c r="C70" s="4"/>
+      <c r="D70" s="1"/>
+      <c r="E70" s="2"/>
+      <c r="F70" s="2"/>
+      <c r="G70" s="4"/>
+    </row>
+    <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A71" s="2"/>
       <c r="B71" s="2"/>
-    </row>
-    <row r="72" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C71" s="4"/>
+      <c r="D71" s="1"/>
+      <c r="E71" s="2"/>
+      <c r="F71" s="2"/>
+      <c r="G71" s="4"/>
+    </row>
+    <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="2"/>
-      <c r="B72" s="5"/>
-    </row>
-    <row r="73" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A73" s="5"/>
+      <c r="B72" s="2"/>
+      <c r="C72" s="4"/>
+      <c r="D72" s="1"/>
+      <c r="E72" s="2"/>
+      <c r="F72" s="2"/>
+      <c r="G72" s="4"/>
+    </row>
+    <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A73" s="2"/>
       <c r="B73" s="2"/>
-    </row>
-    <row r="74" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A74" s="5"/>
+      <c r="C73" s="4"/>
+      <c r="D73" s="1"/>
+      <c r="E73" s="2"/>
+      <c r="F73" s="2"/>
+      <c r="G73" s="4"/>
+    </row>
+    <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A74" s="2"/>
       <c r="B74" s="2"/>
-    </row>
-    <row r="75" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C74" s="4"/>
+      <c r="D74" s="1"/>
+      <c r="E74" s="2"/>
+      <c r="F74" s="2"/>
+      <c r="G74" s="4"/>
+    </row>
+    <row r="75" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="2"/>
-      <c r="B75" s="5"/>
-    </row>
-    <row r="76" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B75" s="2"/>
+      <c r="C75" s="4"/>
+      <c r="D75" s="1"/>
+      <c r="E75" s="2"/>
+      <c r="F75" s="2"/>
+      <c r="G75" s="4"/>
+    </row>
+    <row r="76" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="2"/>
-      <c r="B76" s="5"/>
-    </row>
-    <row r="77" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A77" s="5"/>
+      <c r="B76" s="2"/>
+      <c r="C76" s="4"/>
+      <c r="D76" s="1"/>
+      <c r="E76" s="2"/>
+      <c r="F76" s="2"/>
+      <c r="G76" s="4"/>
+    </row>
+    <row r="77" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A77" s="2"/>
       <c r="B77" s="2"/>
-    </row>
-    <row r="78" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A78" s="5"/>
+      <c r="C77" s="4"/>
+      <c r="D77" s="1"/>
+      <c r="E77" s="2"/>
+      <c r="F77" s="2"/>
+      <c r="G77" s="4"/>
+    </row>
+    <row r="78" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A78" s="2"/>
       <c r="B78" s="2"/>
-    </row>
-    <row r="79" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C78" s="4"/>
+      <c r="D78" s="1"/>
+      <c r="E78" s="2"/>
+      <c r="F78" s="2"/>
+      <c r="G78" s="4"/>
+    </row>
+    <row r="79" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A79" s="2"/>
-      <c r="B79" s="5"/>
+      <c r="B79" s="2"/>
+      <c r="C79" s="4"/>
+      <c r="D79" s="1"/>
+      <c r="E79" s="2"/>
+      <c r="F79" s="2"/>
+      <c r="G79" s="4"/>
+    </row>
+    <row r="80" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A80" s="2"/>
+      <c r="B80" s="2"/>
+      <c r="C80" s="4"/>
+      <c r="D80" s="1"/>
+      <c r="E80" s="2"/>
+      <c r="F80" s="2"/>
+      <c r="G80" s="4"/>
+    </row>
+    <row r="81" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A81" s="2"/>
+      <c r="B81" s="2"/>
+      <c r="C81" s="4"/>
+      <c r="D81" s="1"/>
+      <c r="E81" s="2"/>
+      <c r="F81" s="2"/>
+      <c r="G81" s="4"/>
+    </row>
+    <row r="82" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A82" s="2"/>
+      <c r="B82" s="2"/>
+      <c r="C82" s="4"/>
+      <c r="D82" s="1"/>
+      <c r="E82" s="2"/>
+      <c r="F82" s="2"/>
+      <c r="G82" s="4"/>
+    </row>
+    <row r="83" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A83" s="2"/>
+      <c r="B83" s="2"/>
+      <c r="C83" s="4"/>
+      <c r="D83" s="1"/>
+      <c r="E83" s="2"/>
+      <c r="F83" s="2"/>
+      <c r="G83" s="4"/>
+    </row>
+    <row r="84" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A84" s="2"/>
+      <c r="B84" s="2"/>
+      <c r="C84" s="4"/>
+      <c r="D84" s="1"/>
+      <c r="E84" s="2"/>
+      <c r="F84" s="2"/>
+      <c r="G84" s="4"/>
+    </row>
+    <row r="85" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A85" s="2"/>
+      <c r="B85" s="2"/>
+      <c r="C85" s="4"/>
+      <c r="D85" s="1"/>
+      <c r="E85" s="2"/>
+      <c r="F85" s="2"/>
+      <c r="G85" s="4"/>
+    </row>
+    <row r="86" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A86" s="2"/>
+      <c r="B86" s="2"/>
+      <c r="C86" s="4"/>
+      <c r="D86" s="1"/>
+      <c r="E86" s="2"/>
+      <c r="F86" s="2"/>
+      <c r="G86" s="4"/>
+    </row>
+    <row r="87" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A87" s="2"/>
+      <c r="B87" s="2"/>
+      <c r="C87" s="4"/>
+      <c r="D87" s="1"/>
+      <c r="E87" s="2"/>
+      <c r="F87" s="2"/>
+      <c r="G87" s="4"/>
+    </row>
+    <row r="88" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A88" s="2"/>
+      <c r="B88" s="2"/>
+      <c r="C88" s="4"/>
+      <c r="D88" s="1"/>
+      <c r="E88" s="2"/>
+      <c r="F88" s="2"/>
+      <c r="G88" s="4"/>
+    </row>
+    <row r="89" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A89" s="2"/>
+      <c r="B89" s="2"/>
+      <c r="C89" s="4"/>
+      <c r="D89" s="1"/>
+      <c r="E89" s="2"/>
+      <c r="F89" s="2"/>
+      <c r="G89" s="4"/>
+    </row>
+    <row r="90" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A90" s="2"/>
+      <c r="B90" s="2"/>
+      <c r="C90" s="4"/>
+      <c r="D90" s="1"/>
+      <c r="E90" s="2"/>
+      <c r="F90" s="2"/>
+      <c r="G90" s="4"/>
+    </row>
+    <row r="91" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A91" s="2"/>
+      <c r="B91" s="2"/>
+      <c r="C91" s="4"/>
+      <c r="D91" s="1"/>
+      <c r="E91" s="2"/>
+      <c r="F91" s="2"/>
+      <c r="G91" s="4"/>
+    </row>
+    <row r="92" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A92" s="2"/>
+      <c r="B92" s="2"/>
+      <c r="C92" s="4"/>
+      <c r="D92" s="1"/>
+      <c r="E92" s="2"/>
+      <c r="F92" s="2"/>
+      <c r="G92" s="4"/>
+    </row>
+    <row r="93" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A93" s="2"/>
+      <c r="B93" s="2"/>
+      <c r="C93" s="4"/>
+      <c r="D93" s="1"/>
+      <c r="E93" s="2"/>
+      <c r="F93" s="2"/>
+      <c r="G93" s="4"/>
+    </row>
+    <row r="94" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A94" s="2"/>
+      <c r="B94" s="2"/>
+      <c r="C94" s="4"/>
+      <c r="D94" s="1"/>
+      <c r="E94" s="2"/>
+      <c r="F94" s="2"/>
+      <c r="G94" s="4"/>
+    </row>
+    <row r="95" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A95" s="2"/>
+      <c r="B95" s="2"/>
+      <c r="C95" s="4"/>
+      <c r="D95" s="1"/>
+      <c r="E95" s="2"/>
+      <c r="F95" s="2"/>
+      <c r="G95" s="4"/>
+    </row>
+    <row r="96" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A96" s="2"/>
+      <c r="B96" s="2"/>
+      <c r="C96" s="4"/>
+      <c r="D96" s="1"/>
+      <c r="E96" s="2"/>
+      <c r="F96" s="2"/>
+      <c r="G96" s="4"/>
+    </row>
+    <row r="97" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A97" s="2"/>
+      <c r="B97" s="2"/>
+      <c r="C97" s="4"/>
+      <c r="D97" s="1"/>
+      <c r="E97" s="2"/>
+      <c r="F97" s="2"/>
+      <c r="G97" s="4"/>
+    </row>
+    <row r="98" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A98" s="2"/>
+      <c r="B98" s="2"/>
+      <c r="C98" s="4"/>
+      <c r="D98" s="1"/>
+      <c r="E98" s="2"/>
+      <c r="F98" s="2"/>
+      <c r="G98" s="4"/>
+    </row>
+    <row r="99" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A99" s="2"/>
+      <c r="B99" s="2"/>
+      <c r="C99" s="4"/>
+      <c r="D99" s="1"/>
+      <c r="E99" s="2"/>
+      <c r="F99" s="2"/>
+      <c r="G99" s="4"/>
+    </row>
+    <row r="100" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A100" s="2"/>
+      <c r="B100" s="2"/>
+      <c r="C100" s="4"/>
+      <c r="D100" s="1"/>
+      <c r="E100" s="2"/>
+      <c r="F100" s="2"/>
+      <c r="G100" s="4"/>
+    </row>
+    <row r="101" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A101" s="2"/>
+      <c r="B101" s="2"/>
+      <c r="C101" s="4"/>
+      <c r="D101" s="1"/>
+      <c r="E101" s="2"/>
+      <c r="F101" s="2"/>
+      <c r="G101" s="4"/>
+    </row>
+    <row r="102" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A102" s="2"/>
+      <c r="B102" s="2"/>
+      <c r="C102" s="4"/>
+      <c r="D102" s="1"/>
+      <c r="E102" s="2"/>
+      <c r="F102" s="2"/>
+      <c r="G102" s="4"/>
+    </row>
+    <row r="103" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A103" s="2"/>
+      <c r="B103" s="2"/>
+      <c r="C103" s="4"/>
+      <c r="D103" s="1"/>
+      <c r="E103" s="2"/>
+      <c r="F103" s="2"/>
+      <c r="G103" s="4"/>
+    </row>
+    <row r="104" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A104" s="2"/>
+      <c r="B104" s="2"/>
+      <c r="C104" s="4"/>
+      <c r="D104" s="1"/>
+      <c r="E104" s="2"/>
+      <c r="F104" s="2"/>
+      <c r="G104" s="4"/>
+    </row>
+    <row r="105" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A105" s="2"/>
+      <c r="B105" s="2"/>
+      <c r="C105" s="4"/>
+      <c r="D105" s="1"/>
+      <c r="E105" s="2"/>
+      <c r="F105" s="2"/>
+      <c r="G105" s="4"/>
+    </row>
+    <row r="106" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A106" s="2"/>
+      <c r="B106" s="2"/>
+      <c r="C106" s="4"/>
+      <c r="D106" s="1"/>
+      <c r="E106" s="2"/>
+      <c r="F106" s="2"/>
+      <c r="G106" s="4"/>
+    </row>
+    <row r="107" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A107" s="2"/>
+      <c r="B107" s="2"/>
+      <c r="C107" s="4"/>
+      <c r="D107" s="1"/>
+      <c r="E107" s="2"/>
+      <c r="F107" s="2"/>
+      <c r="G107" s="4"/>
+    </row>
+    <row r="108" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A108" s="2"/>
+      <c r="B108" s="2"/>
+      <c r="C108" s="4"/>
+      <c r="D108" s="1"/>
+      <c r="E108" s="2"/>
+      <c r="F108" s="2"/>
+      <c r="G108" s="4"/>
+    </row>
+    <row r="109" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A109" s="2"/>
+      <c r="B109" s="2"/>
+      <c r="C109" s="4"/>
+      <c r="D109" s="1"/>
+      <c r="E109" s="2"/>
+      <c r="F109" s="2"/>
+      <c r="G109" s="4"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>